<commit_message>
add seg_interval option to evaluate.py
</commit_message>
<xml_diff>
--- a/logs/gma-craft-sintel-shift-110720.xlsx
+++ b/logs/gma-craft-sintel-shift-110720.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\ihpc\motion\craft\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\ihpc\motion\craft\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EDCE96-F9A0-4D9D-888B-D00E90C09168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE944F1-349E-4C2F-B3FA-83EB5D9E97AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06A6EC30-F715-41C1-9B54-00F43650299A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06A6EC30-F715-41C1-9B54-00F43650299A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,15 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>GMA</t>
-  </si>
-  <si>
-    <t>Clean</t>
-  </si>
-  <si>
-    <t>Final</t>
   </si>
   <si>
     <t>CRAFT-nopos</t>
@@ -49,10 +43,19 @@
     <t>CRAFT</t>
   </si>
   <si>
-    <t>Slowflow, 100-3</t>
+    <t>RAFT</t>
   </si>
   <si>
-    <t>Slowflow, 100-9</t>
+    <t>Sintel Clean</t>
+  </si>
+  <si>
+    <t>Sintel Final</t>
+  </si>
+  <si>
+    <t>Slowflow 100-3</t>
+  </si>
+  <si>
+    <t>Slowflow 100-9</t>
   </si>
 </sst>
 </file>
@@ -88,9 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,23 +141,23 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GMA</c:v>
+                  <c:v>RAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:prstDash val="dash"/>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
@@ -169,9 +173,16 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -188,22 +199,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -211,42 +222,49 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$3:$O$3</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$3:$L$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.2200000000000006</c:v>
+                  <c:v>8.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>9.6300000000000008</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.09</c:v>
+                  <c:v>10.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.24</c:v>
+                  <c:v>13.98</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.43</c:v>
+                  <c:v>17.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.67</c:v>
+                  <c:v>25.55</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.07</c:v>
+                  <c:v>36.43</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.21</c:v>
+                  <c:v>69.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.26</c:v>
+                  <c:v>133.26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.790000000000006</c:v>
+                  <c:v>219.51</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>107.62</c:v>
+                  <c:v>293.60000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -264,6 +282,150 @@
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GMA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$4:$L$4</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$4:$L$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.2200000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.43</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.07</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.21</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65.790000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B630-41BC-B16C-B00ED91AB7BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -319,15 +481,22 @@
             <c:bubble3D val="0"/>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-B630-41BC-B16C-B00ED91AB7BC}"/>
+                <c16:uniqueId val="{00000000-C422-4D43-9057-777FB0141054}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -344,22 +513,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -367,7 +536,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$L$4</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$5:$L$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$5:$L$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -410,16 +586,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B630-41BC-B16C-B00ED91AB7BC}"/>
+              <c16:uniqueId val="{00000002-B630-41BC-B16C-B00ED91AB7BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -429,7 +605,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -454,9 +630,16 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -473,22 +656,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -496,7 +679,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$L$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$6:$L$6</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$6:$L$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -539,7 +729,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-B630-41BC-B16C-B00ED91AB7BC}"/>
+              <c16:uniqueId val="{00000002-5379-4F23-863C-F980C679EAE1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -589,16 +779,31 @@
                   </a:rPr>
                   <a:t>Horizontal Shift</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>,</a:t>
-                </a:r>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0">
                     <a:solidFill>
@@ -607,7 +812,7 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t> Sintel Clean</a:t>
+                  <a:t>(a) Sintel Clean</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-SG" sz="1100">
                   <a:solidFill>
@@ -623,8 +828,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.44602887139107611"/>
-              <c:y val="0.90046296296296291"/>
+              <c:x val="0.36547331583552056"/>
+              <c:y val="0.80867801007632667"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -653,7 +858,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -698,6 +903,8 @@
         <c:axId val="1693631168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="150"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -800,7 +1007,7 @@
         </c:txPr>
         <c:crossAx val="1693629920"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -895,11 +1102,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$7</c:f>
+              <c:f>Sheet1!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GMA</c:v>
+                  <c:v>RAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -909,13 +1116,13 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:prstDash val="dash"/>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
@@ -931,9 +1138,16 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -950,22 +1164,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -973,42 +1187,49 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$L$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$8:$O$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$8:$L$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.25</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>10.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.34</c:v>
+                  <c:v>11.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.56</c:v>
+                  <c:v>15.34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.56</c:v>
+                  <c:v>21.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.48</c:v>
+                  <c:v>30.54</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.68</c:v>
+                  <c:v>48.74</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.11</c:v>
+                  <c:v>79.33</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.51</c:v>
+                  <c:v>137.02000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.77</c:v>
+                  <c:v>207.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>83.86</c:v>
+                  <c:v>267.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1025,7 +1246,151 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GMA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$9:$L$9</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$9:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.56</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>83.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7FFC-497F-B48A-C4AE407D73AD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1061,9 +1426,16 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -1080,22 +1452,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1103,7 +1475,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$L$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$10:$L$10</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$10:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1146,16 +1525,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7FFC-497F-B48A-C4AE407D73AD}"/>
+              <c16:uniqueId val="{00000002-7FFC-497F-B48A-C4AE407D73AD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1165,7 +1544,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -1190,9 +1569,16 @@
           </c:marker>
           <c:cat>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$1:$L$1</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -1209,22 +1595,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1232,7 +1618,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$L$9</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$11:$L$11</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1275,7 +1668,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7FFC-497F-B48A-C4AE407D73AD}"/>
+              <c16:uniqueId val="{00000001-1F18-484C-832B-C0DEEC33CFD7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1323,7 +1716,46 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>Horizontal Shift, Sintel Final</a:t>
+                  <a:t>Horizontal Shift</a:t>
+                </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-SG" sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-SG" sz="1100">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>(b) Sintel Final</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1332,8 +1764,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.44602887139107611"/>
-              <c:y val="0.90509259259259256"/>
+              <c:x val="0.36547331583552056"/>
+              <c:y val="0.77344889180519105"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1362,8 +1794,8 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1407,6 +1839,7 @@
         <c:axId val="1693631168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1509,7 +1942,7 @@
         </c:txPr>
         <c:crossAx val="1693629920"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
       </c:valAx>
       <c:spPr>
@@ -1605,11 +2038,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GMA</c:v>
+                  <c:v>RAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1619,13 +2052,13 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:prstDash val="dash"/>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
@@ -1643,7 +2076,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -1660,22 +2093,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1683,42 +2116,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$L$11</c:f>
+              <c:f>Sheet1!$B$13:$L$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>4.6288999999999998</c:v>
+                  <c:v>4.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.0077999999999996</c:v>
+                  <c:v>5.3769</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.4073000000000002</c:v>
+                  <c:v>7.5574000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.7942999999999998</c:v>
+                  <c:v>9.6424000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1615000000000002</c:v>
+                  <c:v>21.307400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.772600000000001</c:v>
+                  <c:v>43.934899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.274000000000001</c:v>
+                  <c:v>85.7179</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57.681800000000003</c:v>
+                  <c:v>165.10599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>109.46980000000001</c:v>
+                  <c:v>247.42420000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>161.97900000000001</c:v>
+                  <c:v>322.36610000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>212.4932</c:v>
+                  <c:v>348.459</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1735,11 +2168,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>Sheet1!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT-nopos</c:v>
+                  <c:v>GMA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1747,8 +2180,139 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$L$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>4.6288999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0077999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.4073000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.7942999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1615000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.772600000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.274000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57.681800000000003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>109.46980000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>161.97900000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>212.4932</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8764-4CFE-A445-B69A906FE633}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRAFT-nopos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
+              <a:prstDash val="dashDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1772,7 +2336,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -1789,22 +2353,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1812,7 +2376,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$L$12</c:f>
+              <c:f>Sheet1!$B$15:$L$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1855,16 +2419,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8764-4CFE-A445-B69A906FE633}"/>
+              <c16:uniqueId val="{00000003-8764-4CFE-A445-B69A906FE633}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>Sheet1!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1874,7 +2438,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -1901,7 +2465,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -1918,22 +2482,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -1941,7 +2505,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$L$13</c:f>
+              <c:f>Sheet1!$B$16:$L$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1984,7 +2548,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-8764-4CFE-A445-B69A906FE633}"/>
+              <c16:uniqueId val="{00000005-8764-4CFE-A445-B69A906FE633}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2034,16 +2598,31 @@
                   </a:rPr>
                   <a:t>Horizontal Shift</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>,</a:t>
-                </a:r>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0">
                     <a:solidFill>
@@ -2052,7 +2631,7 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t> Slowflow 100-3</a:t>
+                  <a:t>(a) Slow Flow 100-3</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-SG" sz="1100">
                   <a:solidFill>
@@ -2068,8 +2647,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.2821399825021873"/>
-              <c:y val="0.90046296296296291"/>
+              <c:x val="0.39880664916885389"/>
+              <c:y val="0.7688192621755614"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2098,7 +2677,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2143,6 +2722,7 @@
         <c:axId val="1693631168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2245,7 +2825,7 @@
         </c:txPr>
         <c:crossAx val="1693629920"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2340,11 +2920,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
+              <c:f>Sheet1!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GMA</c:v>
+                  <c:v>RAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2354,13 +2934,13 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:prstDash val="dash"/>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="diamond"/>
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
@@ -2378,7 +2958,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -2395,22 +2975,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -2418,42 +2998,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$L$15</c:f>
+              <c:f>Sheet1!$B$18:$L$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>6.1040999999999999</c:v>
+                  <c:v>6.4588000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4531999999999998</c:v>
+                  <c:v>6.8236999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.742</c:v>
+                  <c:v>7.9984000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1778000000000004</c:v>
+                  <c:v>11.638199999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.302199999999999</c:v>
+                  <c:v>35.913600000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.805099999999999</c:v>
+                  <c:v>58.421799999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.005899999999997</c:v>
+                  <c:v>98.519300000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>66.088999999999999</c:v>
+                  <c:v>170.7955</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>127.04949999999999</c:v>
+                  <c:v>258.77449999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>174.7276</c:v>
+                  <c:v>312.71789999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>226.12459999999999</c:v>
+                  <c:v>349.65800000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2470,17 +3050,147 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$16</c:f>
+              <c:f>Sheet1!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT-nopos</c:v>
+                  <c:v>GMA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$L$1</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$19:$L$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>6.1040999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4531999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.742</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1778000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19.302199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.805099999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>49.005899999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66.088999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>127.04949999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>174.7276</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>226.12459999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-08C5-4822-A26A-A5193FCFC3CA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CRAFT-nopos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -2508,7 +3218,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -2525,22 +3235,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -2548,7 +3258,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$L$16</c:f>
+              <c:f>Sheet1!$B$20:$L$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2591,16 +3301,16 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-08C5-4822-A26A-A5193FCFC3CA}"/>
+              <c16:uniqueId val="{00000002-08C5-4822-A26A-A5193FCFC3CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$17</c:f>
+              <c:f>Sheet1!$A$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2610,7 +3320,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -2638,7 +3348,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$1:$L$1</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
@@ -2655,22 +3365,22 @@
                 <c:pt idx="4">
                   <c:v>180</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="#,##0">
+                <c:pt idx="5">
                   <c:v>200</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="#,##0">
+                <c:pt idx="6">
                   <c:v>220</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="#,##0">
+                <c:pt idx="7">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="#,##0">
+                <c:pt idx="8">
                   <c:v>260</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="#,##0">
+                <c:pt idx="9">
                   <c:v>280</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="#,##0">
+                <c:pt idx="10">
                   <c:v>300</c:v>
                 </c:pt>
               </c:numCache>
@@ -2678,7 +3388,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$L$17</c:f>
+              <c:f>Sheet1!$B$21:$L$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2721,7 +3431,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-08C5-4822-A26A-A5193FCFC3CA}"/>
+              <c16:uniqueId val="{00000004-08C5-4822-A26A-A5193FCFC3CA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2771,16 +3481,31 @@
                   </a:rPr>
                   <a:t>Horizontal Shift</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1100">
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                  </a:rPr>
-                  <a:t>,</a:t>
-                </a:r>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="1100">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:defRPr>
+                </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1100" baseline="0">
                     <a:solidFill>
@@ -2789,7 +3514,7 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t> Slowflow 100-9</a:t>
+                  <a:t>(b) Slow Flow 100-9</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-SG" sz="1100">
                   <a:solidFill>
@@ -2805,8 +3530,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.2821399825021873"/>
-              <c:y val="0.90046296296296291"/>
+              <c:x val="0.39602887139107618"/>
+              <c:y val="0.7688192621755614"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2835,7 +3560,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2880,6 +3605,7 @@
         <c:axId val="1693631168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2982,7 +3708,7 @@
         </c:txPr>
         <c:crossAx val="1693629920"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5280,16 +6006,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5316,16 +6042,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5356,13 +6082,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5393,15 +6119,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5728,209 +6454,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6FF8DA-B4AA-4326-A020-51F3D0E4BB8B}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1">
+      <c r="B1" s="2">
         <v>100</v>
       </c>
-      <c r="C1">
+      <c r="C1" s="2">
         <v>120</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="2">
         <v>140</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="2">
         <v>160</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="2">
         <v>180</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="2">
         <v>200</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="2">
         <v>220</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="2">
         <v>240</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="2">
         <v>260</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="2">
         <v>280</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="2">
         <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>8.2200000000000006</v>
+        <v>8.48</v>
       </c>
       <c r="C3">
-        <v>9.1999999999999993</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="D3">
-        <v>10.09</v>
+        <v>10.86</v>
       </c>
       <c r="E3">
-        <v>11.24</v>
+        <v>13.98</v>
       </c>
       <c r="F3">
-        <v>12.43</v>
+        <v>17.7</v>
       </c>
       <c r="G3">
-        <v>13.67</v>
+        <v>25.55</v>
       </c>
       <c r="H3">
-        <v>17.07</v>
+        <v>36.43</v>
       </c>
       <c r="I3">
-        <v>21.21</v>
+        <v>69.75</v>
       </c>
       <c r="J3">
-        <v>35.26</v>
+        <v>133.26</v>
       </c>
       <c r="K3">
-        <v>65.790000000000006</v>
+        <v>219.51</v>
       </c>
       <c r="L3">
-        <v>107.62</v>
+        <v>293.60000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B4">
-        <v>8.24</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="C4">
-        <v>9.23</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D4">
-        <v>10.1</v>
+        <v>10.09</v>
       </c>
       <c r="E4">
-        <v>10.89</v>
+        <v>11.24</v>
       </c>
       <c r="F4">
-        <v>11.65</v>
+        <v>12.43</v>
       </c>
       <c r="G4">
-        <v>12.6</v>
+        <v>13.67</v>
       </c>
       <c r="H4">
-        <v>13.66</v>
+        <v>17.07</v>
       </c>
       <c r="I4">
-        <v>15.48</v>
+        <v>21.21</v>
       </c>
       <c r="J4">
-        <v>18.41</v>
+        <v>35.26</v>
       </c>
       <c r="K4">
-        <v>24.84</v>
+        <v>65.790000000000006</v>
       </c>
       <c r="L4">
-        <v>38.020000000000003</v>
+        <v>107.62</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>8.1999999999999993</v>
+        <v>8.24</v>
       </c>
       <c r="C5">
-        <v>9.1999999999999993</v>
+        <v>9.23</v>
       </c>
       <c r="D5">
-        <v>10.08</v>
+        <v>10.1</v>
       </c>
       <c r="E5">
-        <v>10.86</v>
+        <v>10.89</v>
       </c>
       <c r="F5">
-        <v>11.59</v>
+        <v>11.65</v>
       </c>
       <c r="G5">
-        <v>12.38</v>
+        <v>12.6</v>
       </c>
       <c r="H5">
-        <v>13.29</v>
+        <v>13.66</v>
       </c>
       <c r="I5">
-        <v>14.75</v>
+        <v>15.48</v>
       </c>
       <c r="J5">
-        <v>16.72</v>
+        <v>18.41</v>
       </c>
       <c r="K5">
-        <v>20.74</v>
+        <v>24.84</v>
       </c>
       <c r="L5">
-        <v>30.65</v>
+        <v>38.020000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
+      <c r="B6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C6">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="D6">
+        <v>10.08</v>
+      </c>
+      <c r="E6">
+        <v>10.86</v>
+      </c>
+      <c r="F6">
+        <v>11.59</v>
+      </c>
+      <c r="G6">
+        <v>12.38</v>
+      </c>
+      <c r="H6">
+        <v>13.29</v>
+      </c>
+      <c r="I6">
+        <v>14.75</v>
+      </c>
+      <c r="J6">
+        <v>16.72</v>
+      </c>
+      <c r="K6">
+        <v>20.74</v>
+      </c>
+      <c r="L6">
+        <v>30.65</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>8.25</v>
-      </c>
-      <c r="C7">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="D7">
-        <v>10.34</v>
-      </c>
-      <c r="E7">
-        <v>11.56</v>
-      </c>
-      <c r="F7">
-        <v>12.56</v>
-      </c>
-      <c r="G7">
-        <v>14.48</v>
-      </c>
-      <c r="H7">
-        <v>16.68</v>
-      </c>
-      <c r="I7">
-        <v>21.11</v>
-      </c>
-      <c r="J7">
-        <v>35.51</v>
-      </c>
-      <c r="K7">
-        <v>52.77</v>
-      </c>
-      <c r="L7">
-        <v>83.86</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5938,317 +6670,470 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>8.2799999999999994</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C8">
-        <v>9.2200000000000006</v>
+        <v>10.18</v>
       </c>
       <c r="D8">
-        <v>10.26</v>
+        <v>11.76</v>
       </c>
       <c r="E8">
-        <v>11.06</v>
+        <v>15.34</v>
       </c>
       <c r="F8">
-        <v>11.97</v>
+        <v>21.4</v>
       </c>
       <c r="G8">
-        <v>12.97</v>
+        <v>30.54</v>
       </c>
       <c r="H8">
-        <v>13.89</v>
+        <v>48.74</v>
       </c>
       <c r="I8">
-        <v>17.27</v>
+        <v>79.33</v>
       </c>
       <c r="J8">
-        <v>23.61</v>
+        <v>137.02000000000001</v>
       </c>
       <c r="K8">
-        <v>35.54</v>
+        <v>207.5</v>
       </c>
       <c r="L8">
-        <v>47.08</v>
+        <v>267.26</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B9">
-        <v>8.3000000000000007</v>
+        <v>8.25</v>
       </c>
       <c r="C9">
-        <v>9.2799999999999994</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D9">
-        <v>10.11</v>
+        <v>10.34</v>
       </c>
       <c r="E9">
-        <v>11.01</v>
+        <v>11.56</v>
       </c>
       <c r="F9">
-        <v>11.85</v>
+        <v>12.56</v>
       </c>
       <c r="G9">
-        <v>12.56</v>
+        <v>14.48</v>
       </c>
       <c r="H9">
-        <v>13.63</v>
+        <v>16.68</v>
       </c>
       <c r="I9">
-        <v>15.97</v>
+        <v>21.11</v>
       </c>
       <c r="J9">
-        <v>20.59</v>
+        <v>35.51</v>
       </c>
       <c r="K9">
-        <v>27.27</v>
+        <v>52.77</v>
       </c>
       <c r="L9">
-        <v>50.77</v>
+        <v>83.86</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="C10">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="D10">
+        <v>10.26</v>
+      </c>
+      <c r="E10">
+        <v>11.06</v>
+      </c>
+      <c r="F10">
+        <v>11.97</v>
+      </c>
+      <c r="G10">
+        <v>12.97</v>
+      </c>
+      <c r="H10">
+        <v>13.89</v>
+      </c>
+      <c r="I10">
+        <v>17.27</v>
+      </c>
+      <c r="J10">
+        <v>23.61</v>
+      </c>
+      <c r="K10">
+        <v>35.54</v>
+      </c>
+      <c r="L10">
+        <v>47.08</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>4.6288999999999998</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="C11">
-        <v>5.0077999999999996</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="D11">
-        <v>5.4073000000000002</v>
+        <v>10.11</v>
       </c>
       <c r="E11">
-        <v>5.7942999999999998</v>
+        <v>11.01</v>
       </c>
       <c r="F11">
-        <v>7.1615000000000002</v>
+        <v>11.85</v>
       </c>
       <c r="G11">
-        <v>12.772600000000001</v>
+        <v>12.56</v>
       </c>
       <c r="H11">
-        <v>26.274000000000001</v>
+        <v>13.63</v>
       </c>
       <c r="I11">
-        <v>57.681800000000003</v>
+        <v>15.97</v>
       </c>
       <c r="J11">
-        <v>109.46980000000001</v>
+        <v>20.59</v>
       </c>
       <c r="K11">
-        <v>161.97900000000001</v>
+        <v>27.27</v>
       </c>
       <c r="L11">
-        <v>212.4932</v>
+        <v>50.77</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>4.6178999999999997</v>
-      </c>
-      <c r="C12">
-        <v>5.1176000000000004</v>
-      </c>
-      <c r="D12">
-        <v>5.4577999999999998</v>
-      </c>
-      <c r="E12">
-        <v>5.8444000000000003</v>
-      </c>
-      <c r="F12">
-        <v>6.9322999999999997</v>
-      </c>
-      <c r="G12">
-        <v>7.3428000000000004</v>
-      </c>
-      <c r="H12">
-        <v>11.3188</v>
-      </c>
-      <c r="I12">
-        <v>17.174800000000001</v>
-      </c>
-      <c r="J12">
-        <v>21.888300000000001</v>
-      </c>
-      <c r="K12">
-        <v>39.525300000000001</v>
-      </c>
-      <c r="L12">
-        <v>74.785399999999996</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>4.6582999999999997</v>
+        <v>4.79</v>
       </c>
       <c r="C13">
-        <v>5.1035000000000004</v>
+        <v>5.3769</v>
       </c>
       <c r="D13">
-        <v>5.48</v>
+        <v>7.5574000000000003</v>
       </c>
       <c r="E13">
-        <v>5.8604000000000003</v>
+        <v>9.6424000000000003</v>
       </c>
       <c r="F13">
-        <v>6.8990999999999998</v>
+        <v>21.307400000000001</v>
       </c>
       <c r="G13">
-        <v>7.8916000000000004</v>
+        <v>43.934899999999999</v>
       </c>
       <c r="H13">
-        <v>8.7934000000000001</v>
+        <v>85.7179</v>
       </c>
       <c r="I13">
-        <v>15.683299999999999</v>
+        <v>165.10599999999999</v>
       </c>
       <c r="J13">
-        <v>18.7315</v>
+        <v>247.42420000000001</v>
       </c>
       <c r="K13">
-        <v>42.9831</v>
+        <v>322.36610000000002</v>
       </c>
       <c r="L13">
-        <v>74.621799999999993</v>
+        <v>348.459</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>4.6288999999999998</v>
+      </c>
+      <c r="C14">
+        <v>5.0077999999999996</v>
+      </c>
+      <c r="D14">
+        <v>5.4073000000000002</v>
+      </c>
+      <c r="E14">
+        <v>5.7942999999999998</v>
+      </c>
+      <c r="F14">
+        <v>7.1615000000000002</v>
+      </c>
+      <c r="G14">
+        <v>12.772600000000001</v>
+      </c>
+      <c r="H14">
+        <v>26.274000000000001</v>
+      </c>
+      <c r="I14">
+        <v>57.681800000000003</v>
+      </c>
+      <c r="J14">
+        <v>109.46980000000001</v>
+      </c>
+      <c r="K14">
+        <v>161.97900000000001</v>
+      </c>
+      <c r="L14">
+        <v>212.4932</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15">
-        <v>6.1040999999999999</v>
+        <v>4.6178999999999997</v>
       </c>
       <c r="C15">
-        <v>6.4531999999999998</v>
+        <v>5.1176000000000004</v>
       </c>
       <c r="D15">
-        <v>6.742</v>
+        <v>5.4577999999999998</v>
       </c>
       <c r="E15">
-        <v>7.1778000000000004</v>
+        <v>5.8444000000000003</v>
       </c>
       <c r="F15">
-        <v>19.302199999999999</v>
+        <v>6.9322999999999997</v>
       </c>
       <c r="G15">
-        <v>24.805099999999999</v>
+        <v>7.3428000000000004</v>
       </c>
       <c r="H15">
-        <v>49.005899999999997</v>
+        <v>11.3188</v>
       </c>
       <c r="I15">
-        <v>66.088999999999999</v>
+        <v>17.174800000000001</v>
       </c>
       <c r="J15">
-        <v>127.04949999999999</v>
+        <v>21.888300000000001</v>
       </c>
       <c r="K15">
-        <v>174.7276</v>
+        <v>39.525300000000001</v>
       </c>
       <c r="L15">
-        <v>226.12459999999999</v>
+        <v>74.785399999999996</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>6.1260000000000003</v>
+        <v>4.6582999999999997</v>
       </c>
       <c r="C16">
-        <v>6.4550000000000001</v>
+        <v>5.1035000000000004</v>
       </c>
       <c r="D16">
-        <v>6.7648000000000001</v>
+        <v>5.48</v>
       </c>
       <c r="E16">
-        <v>7.0918999999999999</v>
+        <v>5.8604000000000003</v>
       </c>
       <c r="F16">
-        <v>8.4631000000000007</v>
+        <v>6.8990999999999998</v>
       </c>
       <c r="G16">
-        <v>10.1149</v>
+        <v>7.8916000000000004</v>
       </c>
       <c r="H16">
-        <v>14.0595</v>
+        <v>8.7934000000000001</v>
       </c>
       <c r="I16">
-        <v>17.566099999999999</v>
+        <v>15.683299999999999</v>
       </c>
       <c r="J16">
-        <v>29.749300000000002</v>
+        <v>18.7315</v>
       </c>
       <c r="K16">
-        <v>49.259500000000003</v>
+        <v>42.9831</v>
       </c>
       <c r="L16">
-        <v>77.055899999999994</v>
+        <v>74.621799999999993</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>6.4588000000000001</v>
+      </c>
+      <c r="C18">
+        <v>6.8236999999999997</v>
+      </c>
+      <c r="D18">
+        <v>7.9984000000000002</v>
+      </c>
+      <c r="E18">
+        <v>11.638199999999999</v>
+      </c>
+      <c r="F18">
+        <v>35.913600000000002</v>
+      </c>
+      <c r="G18">
+        <v>58.421799999999998</v>
+      </c>
+      <c r="H18">
+        <v>98.519300000000001</v>
+      </c>
+      <c r="I18">
+        <v>170.7955</v>
+      </c>
+      <c r="J18">
+        <v>258.77449999999999</v>
+      </c>
+      <c r="K18">
+        <v>312.71789999999999</v>
+      </c>
+      <c r="L18">
+        <v>349.65800000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>6.1040999999999999</v>
+      </c>
+      <c r="C19">
+        <v>6.4531999999999998</v>
+      </c>
+      <c r="D19">
+        <v>6.742</v>
+      </c>
+      <c r="E19">
+        <v>7.1778000000000004</v>
+      </c>
+      <c r="F19">
+        <v>19.302199999999999</v>
+      </c>
+      <c r="G19">
+        <v>24.805099999999999</v>
+      </c>
+      <c r="H19">
+        <v>49.005899999999997</v>
+      </c>
+      <c r="I19">
+        <v>66.088999999999999</v>
+      </c>
+      <c r="J19">
+        <v>127.04949999999999</v>
+      </c>
+      <c r="K19">
+        <v>174.7276</v>
+      </c>
+      <c r="L19">
+        <v>226.12459999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>6.1260000000000003</v>
+      </c>
+      <c r="C20">
+        <v>6.4550000000000001</v>
+      </c>
+      <c r="D20">
+        <v>6.7648000000000001</v>
+      </c>
+      <c r="E20">
+        <v>7.0918999999999999</v>
+      </c>
+      <c r="F20">
+        <v>8.4631000000000007</v>
+      </c>
+      <c r="G20">
+        <v>10.1149</v>
+      </c>
+      <c r="H20">
+        <v>14.0595</v>
+      </c>
+      <c r="I20">
+        <v>17.566099999999999</v>
+      </c>
+      <c r="J20">
+        <v>29.749300000000002</v>
+      </c>
+      <c r="K20">
+        <v>49.259500000000003</v>
+      </c>
+      <c r="L20">
+        <v>77.055899999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
         <v>6.0511999999999997</v>
       </c>
-      <c r="C17">
+      <c r="C21">
         <v>6.4711999999999996</v>
       </c>
-      <c r="D17">
+      <c r="D21">
         <v>6.8167</v>
       </c>
-      <c r="E17">
+      <c r="E21">
         <v>7.9703999999999997</v>
       </c>
-      <c r="F17">
+      <c r="F21">
         <v>8.7040000000000006</v>
       </c>
-      <c r="G17">
+      <c r="G21">
         <v>10.4579</v>
       </c>
-      <c r="H17">
+      <c r="H21">
         <v>17.0823</v>
       </c>
-      <c r="I17">
+      <c r="I21">
         <v>17.972999999999999</v>
       </c>
-      <c r="J17">
+      <c r="J21">
         <v>22.9312</v>
       </c>
-      <c r="K17">
+      <c r="K21">
         <v>43.205300000000001</v>
       </c>
-      <c r="L17">
+      <c r="L21">
         <v>92.832499999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update shifted image evaluation results
</commit_message>
<xml_diff>
--- a/logs/gma-craft-sintel-shift-110720.xlsx
+++ b/logs/gma-craft-sintel-shift-110720.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\ihpc\motion\craft\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560892F9-F673-44FC-8F27-20D424411C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E6BF7-A156-4B27-BD7B-D567D5ED8682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{06A6EC30-F715-41C1-9B54-00F43650299A}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>GMA</t>
   </si>
   <si>
-    <t>CRAFT-nopos</t>
-  </si>
-  <si>
     <t>CRAFT</t>
   </si>
   <si>
@@ -56,6 +53,9 @@
   </si>
   <si>
     <t>Slowflow 100-9</t>
+  </si>
+  <si>
+    <t>CRAFT-pos</t>
   </si>
 </sst>
 </file>
@@ -234,37 +234,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.48</c:v>
+                  <c:v>1.1953879999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6300000000000008</c:v>
+                  <c:v>1.431732</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.86</c:v>
+                  <c:v>1.905853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.98</c:v>
+                  <c:v>4.3757539999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.7</c:v>
+                  <c:v>7.9348369999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.55</c:v>
+                  <c:v>15.927391</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.43</c:v>
+                  <c:v>27.272524000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>69.75</c:v>
+                  <c:v>62.614623999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>133.26</c:v>
+                  <c:v>129.051132</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>219.51</c:v>
+                  <c:v>215.87803600000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>293.60000000000002</c:v>
+                  <c:v>292.40774499999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -378,37 +378,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.2200000000000006</c:v>
+                  <c:v>0.76826300000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>0.81113000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.09</c:v>
+                  <c:v>0.84672800000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.24</c:v>
+                  <c:v>1.1146149999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.43</c:v>
+                  <c:v>2.2158030000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.67</c:v>
+                  <c:v>2.7051310000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.07</c:v>
+                  <c:v>5.5252239999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.21</c:v>
+                  <c:v>10.78711</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.26</c:v>
+                  <c:v>26.931463000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.790000000000006</c:v>
+                  <c:v>65.862610000000004</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>107.62</c:v>
+                  <c:v>122.669167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -429,7 +429,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT-nopos</c:v>
+                  <c:v>CRAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -548,37 +548,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.24</c:v>
+                  <c:v>0.78029400000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.23</c:v>
+                  <c:v>0.80618100000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.1</c:v>
+                  <c:v>0.81948100000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.89</c:v>
+                  <c:v>0.84702</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.65</c:v>
+                  <c:v>0.93210499999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.6</c:v>
+                  <c:v>1.3161389999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.66</c:v>
+                  <c:v>1.935262</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.48</c:v>
+                  <c:v>3.4459559999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.41</c:v>
+                  <c:v>6.2982769999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.84</c:v>
+                  <c:v>12.852422000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38.020000000000003</c:v>
+                  <c:v>26.952969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -599,7 +599,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT</c:v>
+                  <c:v>CRAFT-pos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -691,37 +691,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.1999999999999993</c:v>
+                  <c:v>0.76139000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>0.80885499999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.08</c:v>
+                  <c:v>0.82048500000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.86</c:v>
+                  <c:v>0.897621</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.59</c:v>
+                  <c:v>0.96037799999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.38</c:v>
+                  <c:v>1.1586590000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.29</c:v>
+                  <c:v>1.532184</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.75</c:v>
+                  <c:v>2.681743</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.72</c:v>
+                  <c:v>4.4309320000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.74</c:v>
+                  <c:v>8.4529910000000008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30.65</c:v>
+                  <c:v>18.661818</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1199,37 +1199,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.8000000000000007</c:v>
+                  <c:v>2.1290529999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.18</c:v>
+                  <c:v>2.7150720000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.76</c:v>
+                  <c:v>3.6476410000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.34</c:v>
+                  <c:v>6.8839370000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.4</c:v>
+                  <c:v>12.736933000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.54</c:v>
+                  <c:v>22.282800999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48.74</c:v>
+                  <c:v>41.147686</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79.33</c:v>
+                  <c:v>73.385955999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>137.02000000000001</c:v>
+                  <c:v>133.187805</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>207.5</c:v>
+                  <c:v>205.21159399999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>267.26</c:v>
+                  <c:v>265.45431500000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1343,37 +1343,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.25</c:v>
+                  <c:v>1.307393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1999999999999993</c:v>
+                  <c:v>1.5838669999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.34</c:v>
+                  <c:v>1.9818499999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.56</c:v>
+                  <c:v>2.5614370000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.56</c:v>
+                  <c:v>3.3465229999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.48</c:v>
+                  <c:v>4.6601160000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.68</c:v>
+                  <c:v>6.495285</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.11</c:v>
+                  <c:v>15.410917</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.51</c:v>
+                  <c:v>30.326699999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.77</c:v>
+                  <c:v>55.885406000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>83.86</c:v>
+                  <c:v>100.21272999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1394,7 +1394,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT-nopos</c:v>
+                  <c:v>CRAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1487,37 +1487,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.2799999999999994</c:v>
+                  <c:v>1.354949</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2200000000000006</c:v>
+                  <c:v>1.3846639999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.26</c:v>
+                  <c:v>1.6203829999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.06</c:v>
+                  <c:v>1.7017659999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.97</c:v>
+                  <c:v>1.9758150000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.97</c:v>
+                  <c:v>2.4542549999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.89</c:v>
+                  <c:v>2.933646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.27</c:v>
+                  <c:v>6.1183379999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.61</c:v>
+                  <c:v>12.544663999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.54</c:v>
+                  <c:v>24.818259999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47.08</c:v>
+                  <c:v>36.972304999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1538,7 +1538,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT</c:v>
+                  <c:v>CRAFT-pos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1630,37 +1630,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>1.341348</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.2799999999999994</c:v>
+                  <c:v>1.4010849999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.11</c:v>
+                  <c:v>1.4474560000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.01</c:v>
+                  <c:v>1.6149089999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.85</c:v>
+                  <c:v>1.8939870000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.56</c:v>
+                  <c:v>2.0595119999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.63</c:v>
+                  <c:v>2.714531</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.97</c:v>
+                  <c:v>4.7984660000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.59</c:v>
+                  <c:v>9.3511790000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.27</c:v>
+                  <c:v>16.237572</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>50.77</c:v>
+                  <c:v>40.465496000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1839,7 +1839,7 @@
         <c:axId val="1693631168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
+          <c:max val="120"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2302,7 +2302,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT-nopos</c:v>
+                  <c:v>CRAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2432,7 +2432,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT</c:v>
+                  <c:v>CRAFT-pos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3184,7 +3184,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT-nopos</c:v>
+                  <c:v>CRAFT</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3314,7 +3314,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CRAFT</c:v>
+                  <c:v>CRAFT-pos</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6456,8 +6456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6FF8DA-B4AA-4326-A020-51F3D0E4BB8B}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6499,7 +6499,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -6510,40 +6510,40 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>8.48</v>
+        <v>1.1953879999999999</v>
       </c>
       <c r="C3">
-        <v>9.6300000000000008</v>
+        <v>1.431732</v>
       </c>
       <c r="D3">
-        <v>10.86</v>
+        <v>1.905853</v>
       </c>
       <c r="E3">
-        <v>13.98</v>
+        <v>4.3757539999999997</v>
       </c>
       <c r="F3">
-        <v>17.7</v>
+        <v>7.9348369999999999</v>
       </c>
       <c r="G3">
-        <v>25.55</v>
+        <v>15.927391</v>
       </c>
       <c r="H3">
-        <v>36.43</v>
+        <v>27.272524000000001</v>
       </c>
       <c r="I3">
-        <v>69.75</v>
+        <v>62.614623999999999</v>
       </c>
       <c r="J3">
-        <v>133.26</v>
+        <v>129.051132</v>
       </c>
       <c r="K3">
-        <v>219.51</v>
+        <v>215.87803600000001</v>
       </c>
       <c r="L3">
-        <v>293.60000000000002</v>
+        <v>292.40774499999998</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -6551,37 +6551,37 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>8.2200000000000006</v>
+        <v>0.76826300000000003</v>
       </c>
       <c r="C4">
-        <v>9.1999999999999993</v>
+        <v>0.81113000000000002</v>
       </c>
       <c r="D4">
-        <v>10.09</v>
+        <v>0.84672800000000004</v>
       </c>
       <c r="E4">
-        <v>11.24</v>
+        <v>1.1146149999999999</v>
       </c>
       <c r="F4">
-        <v>12.43</v>
+        <v>2.2158030000000002</v>
       </c>
       <c r="G4">
-        <v>13.67</v>
+        <v>2.7051310000000002</v>
       </c>
       <c r="H4">
-        <v>17.07</v>
+        <v>5.5252239999999997</v>
       </c>
       <c r="I4">
-        <v>21.21</v>
+        <v>10.78711</v>
       </c>
       <c r="J4">
-        <v>35.26</v>
+        <v>26.931463000000001</v>
       </c>
       <c r="K4">
-        <v>65.790000000000006</v>
+        <v>65.862610000000004</v>
       </c>
       <c r="L4">
-        <v>107.62</v>
+        <v>122.669167</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -6589,118 +6589,118 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>8.24</v>
+        <v>0.78029400000000004</v>
       </c>
       <c r="C5">
-        <v>9.23</v>
+        <v>0.80618100000000004</v>
       </c>
       <c r="D5">
-        <v>10.1</v>
+        <v>0.81948100000000001</v>
       </c>
       <c r="E5">
-        <v>10.89</v>
+        <v>0.84702</v>
       </c>
       <c r="F5">
-        <v>11.65</v>
+        <v>0.93210499999999996</v>
       </c>
       <c r="G5">
-        <v>12.6</v>
+        <v>1.3161389999999999</v>
       </c>
       <c r="H5">
-        <v>13.66</v>
+        <v>1.935262</v>
       </c>
       <c r="I5">
-        <v>15.48</v>
+        <v>3.4459559999999998</v>
       </c>
       <c r="J5">
-        <v>18.41</v>
+        <v>6.2982769999999997</v>
       </c>
       <c r="K5">
-        <v>24.84</v>
+        <v>12.852422000000001</v>
       </c>
       <c r="L5">
-        <v>38.020000000000003</v>
+        <v>26.952969</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>8.1999999999999993</v>
+        <v>0.76139000000000001</v>
       </c>
       <c r="C6">
-        <v>9.1999999999999993</v>
+        <v>0.80885499999999999</v>
       </c>
       <c r="D6">
-        <v>10.08</v>
+        <v>0.82048500000000002</v>
       </c>
       <c r="E6">
-        <v>10.86</v>
+        <v>0.897621</v>
       </c>
       <c r="F6">
-        <v>11.59</v>
+        <v>0.96037799999999995</v>
       </c>
       <c r="G6">
-        <v>12.38</v>
+        <v>1.1586590000000001</v>
       </c>
       <c r="H6">
-        <v>13.29</v>
+        <v>1.532184</v>
       </c>
       <c r="I6">
-        <v>14.75</v>
+        <v>2.681743</v>
       </c>
       <c r="J6">
-        <v>16.72</v>
+        <v>4.4309320000000003</v>
       </c>
       <c r="K6">
-        <v>20.74</v>
+        <v>8.4529910000000008</v>
       </c>
       <c r="L6">
-        <v>30.65</v>
+        <v>18.661818</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>8.8000000000000007</v>
+        <v>2.1290529999999999</v>
       </c>
       <c r="C8">
-        <v>10.18</v>
+        <v>2.7150720000000002</v>
       </c>
       <c r="D8">
-        <v>11.76</v>
+        <v>3.6476410000000001</v>
       </c>
       <c r="E8">
-        <v>15.34</v>
+        <v>6.8839370000000004</v>
       </c>
       <c r="F8">
-        <v>21.4</v>
+        <v>12.736933000000001</v>
       </c>
       <c r="G8">
-        <v>30.54</v>
+        <v>22.282800999999999</v>
       </c>
       <c r="H8">
-        <v>48.74</v>
+        <v>41.147686</v>
       </c>
       <c r="I8">
-        <v>79.33</v>
+        <v>73.385955999999993</v>
       </c>
       <c r="J8">
-        <v>137.02000000000001</v>
+        <v>133.187805</v>
       </c>
       <c r="K8">
-        <v>207.5</v>
+        <v>205.21159399999999</v>
       </c>
       <c r="L8">
-        <v>267.26</v>
+        <v>265.45431500000001</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6708,37 +6708,37 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>8.25</v>
+        <v>1.307393</v>
       </c>
       <c r="C9">
-        <v>9.1999999999999993</v>
+        <v>1.5838669999999999</v>
       </c>
       <c r="D9">
-        <v>10.34</v>
+        <v>1.9818499999999999</v>
       </c>
       <c r="E9">
-        <v>11.56</v>
+        <v>2.5614370000000002</v>
       </c>
       <c r="F9">
-        <v>12.56</v>
+        <v>3.3465229999999999</v>
       </c>
       <c r="G9">
-        <v>14.48</v>
+        <v>4.6601160000000004</v>
       </c>
       <c r="H9">
-        <v>16.68</v>
+        <v>6.495285</v>
       </c>
       <c r="I9">
-        <v>21.11</v>
+        <v>15.410917</v>
       </c>
       <c r="J9">
-        <v>35.51</v>
+        <v>30.326699999999999</v>
       </c>
       <c r="K9">
-        <v>52.77</v>
+        <v>55.885406000000003</v>
       </c>
       <c r="L9">
-        <v>83.86</v>
+        <v>100.21272999999999</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -6746,85 +6746,85 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>8.2799999999999994</v>
+        <v>1.354949</v>
       </c>
       <c r="C10">
-        <v>9.2200000000000006</v>
+        <v>1.3846639999999999</v>
       </c>
       <c r="D10">
-        <v>10.26</v>
+        <v>1.6203829999999999</v>
       </c>
       <c r="E10">
-        <v>11.06</v>
+        <v>1.7017659999999999</v>
       </c>
       <c r="F10">
-        <v>11.97</v>
+        <v>1.9758150000000001</v>
       </c>
       <c r="G10">
-        <v>12.97</v>
+        <v>2.4542549999999999</v>
       </c>
       <c r="H10">
-        <v>13.89</v>
+        <v>2.933646</v>
       </c>
       <c r="I10">
-        <v>17.27</v>
+        <v>6.1183379999999996</v>
       </c>
       <c r="J10">
-        <v>23.61</v>
+        <v>12.544663999999999</v>
       </c>
       <c r="K10">
-        <v>35.54</v>
+        <v>24.818259999999999</v>
       </c>
       <c r="L10">
-        <v>47.08</v>
+        <v>36.972304999999999</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>8.3000000000000007</v>
+        <v>1.341348</v>
       </c>
       <c r="C11">
-        <v>9.2799999999999994</v>
+        <v>1.4010849999999999</v>
       </c>
       <c r="D11">
-        <v>10.11</v>
+        <v>1.4474560000000001</v>
       </c>
       <c r="E11">
-        <v>11.01</v>
+        <v>1.6149089999999999</v>
       </c>
       <c r="F11">
-        <v>11.85</v>
+        <v>1.8939870000000001</v>
       </c>
       <c r="G11">
-        <v>12.56</v>
+        <v>2.0595119999999998</v>
       </c>
       <c r="H11">
-        <v>13.63</v>
+        <v>2.714531</v>
       </c>
       <c r="I11">
-        <v>15.97</v>
+        <v>4.7984660000000003</v>
       </c>
       <c r="J11">
-        <v>20.59</v>
+        <v>9.3511790000000001</v>
       </c>
       <c r="K11">
-        <v>27.27</v>
+        <v>16.237572</v>
       </c>
       <c r="L11">
-        <v>50.77</v>
+        <v>40.465496000000002</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>1.5572999999999999</v>
@@ -6938,7 +6938,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>1.4206000000000001</v>
@@ -6976,12 +6976,12 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18">
         <v>3.8877000000000002</v>
@@ -7095,7 +7095,7 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B21">
         <v>3.5718000000000001</v>

</xml_diff>